<commit_message>
Concluindo o Dicionario de Dados e Fazendo Pequenas Alterações na Modelagem Logica e Fisica do Banco de Dados
</commit_message>
<xml_diff>
--- a/doc/db_docs/dicionario_de_dados/dicionario_de_dados.xlsx
+++ b/doc/db_docs/dicionario_de_dados/dicionario_de_dados.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,13 +11,130 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+  <si>
+    <t>Atributo</t>
+  </si>
+  <si>
+    <t>Nome do campo</t>
+  </si>
+  <si>
+    <t>Tipo de dado</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Restrição</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Numérico inteiro</t>
+  </si>
+  <si>
+    <t>Chave primária</t>
+  </si>
+  <si>
+    <t>Alfanumérico</t>
+  </si>
+  <si>
+    <t>Preenchimento Obrigatorio</t>
+  </si>
+  <si>
+    <t>idUser</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>idScore</t>
+  </si>
+  <si>
+    <t>matchScore</t>
+  </si>
+  <si>
+    <t>fkUser</t>
+  </si>
+  <si>
+    <t>Numérico decimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Bytes
+</t>
+  </si>
+  <si>
+    <t>(9, 2)</t>
+  </si>
+  <si>
+    <t>Chave Estrangeira</t>
+  </si>
+  <si>
+    <t>Numero Maximo Permitido</t>
+  </si>
+  <si>
+    <t>O idUser deverá armazenar 
+um registro numerico para identificar cada Usuario</t>
+  </si>
+  <si>
+    <t>Nome da conta do Usuario dentro do Site</t>
+  </si>
+  <si>
+    <t>Senha da conta do Usuario</t>
+  </si>
+  <si>
+    <t>Email que sera utilizado para o Usuario se Logar no Site</t>
+  </si>
+  <si>
+    <t>lastMatchScore</t>
+  </si>
+  <si>
+    <t>Data e Horario do Dia</t>
+  </si>
+  <si>
+    <t>Data e Hora Consistente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ano-Mês-Dia Hora:Minuto:Segundo
+</t>
+  </si>
+  <si>
+    <t>Tabela de Usuarios (tb_user) - Tabela Forte</t>
+  </si>
+  <si>
+    <t>Tabela de Scores dos Usuarios (tb_player_score) - Tabela Fraca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O idScore deverá armazenar 
+um registro numerico para identificar a pontuação do Jogador   </t>
+  </si>
+  <si>
+    <t>Liga a Pontuação a seu Determinado Jogador na Tabela Usuarios</t>
+  </si>
+  <si>
+    <t>Pontuação do Jogador</t>
+  </si>
+  <si>
+    <t>Momento que esse Registro foi armazenado no Banco de Dados</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +142,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -42,25 +195,401 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +627,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,7 +699,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -343,36 +872,274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
+    <col min="5" max="5" width="76.5703125" customWidth="1"/>
+    <col min="6" max="6" width="82" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4294967295</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="11">
+        <v>80</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A9:F9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nova tela de Finish e Play Again, e alguns ajustes nos documentos
</commit_message>
<xml_diff>
--- a/doc/db_docs/dicionario_de_dados/dicionario_de_dados.xlsx
+++ b/doc/db_docs/dicionario_de_dados/dicionario_de_dados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>Atributo</t>
   </si>
@@ -128,13 +128,16 @@
   </si>
   <si>
     <t>Momento que esse Registro foi armazenado no Banco de Dados</t>
+  </si>
+  <si>
+    <t>Futura Implementação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +163,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -530,24 +552,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -560,16 +564,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,14 +913,14 @@
   <sheetData>
     <row r="1" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -1001,119 +1023,130 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
+      <c r="A9" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D11" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F11" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F14" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+    <row r="15" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F15" s="12" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Melhorando o LLD e o HLD e arrumando pequeno erro no dicionario de dados
</commit_message>
<xml_diff>
--- a/doc/db_docs/dicionario_de_dados/dicionario_de_dados.xlsx
+++ b/doc/db_docs/dicionario_de_dados/dicionario_de_dados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Atributo</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Futura Implementação</t>
+  </si>
+  <si>
+    <t>4 Bytes</t>
   </si>
 </sst>
 </file>
@@ -564,6 +567,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,9 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -898,7 +901,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,14 +916,14 @@
   <sheetData>
     <row r="1" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -952,8 +955,8 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1">
-        <v>4294967295</v>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1024,24 +1027,24 @@
     </row>
     <row r="8" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
@@ -1133,7 +1136,7 @@
       <c r="C15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="11" t="s">

</xml_diff>